<commit_message>
Oppdatert budsjett etter kjøp
</commit_message>
<xml_diff>
--- a/budsjett.xlsx
+++ b/budsjett.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Droneteknologi/3_år/bachelor/bach_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Droneteknologi/3_år/Bachelor/bach_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230C70E-2735-414B-92ED-9C2231244854}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC1C64-2837-0746-8DCA-4084948C9B5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="24460" windowHeight="15460" xr2:uid="{12C7EF9D-573F-4E9A-B276-50794D669FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t xml:space="preserve">Utgifter </t>
   </si>
@@ -54,9 +59,6 @@
     <t>Drone m. frakt</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>FrSky X8R</t>
   </si>
   <si>
@@ -163,16 +165,33 @@
   </si>
   <si>
     <t>Estimert kostnad totalfrakt</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Kjøpt</t>
+  </si>
+  <si>
+    <t>Ikke kjøpt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,10 +241,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -234,8 +254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,7 +573,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -566,32 +588,35 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -603,16 +628,19 @@
         <f t="shared" ref="F3:F13" si="0">D3*E3</f>
         <v>1050</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -624,16 +652,19 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
+      <c r="H4" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -645,16 +676,19 @@
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
-      <c r="H5" t="s">
-        <v>20</v>
+      <c r="H5" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -666,16 +700,19 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="H6" t="s">
-        <v>22</v>
+      <c r="H6" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -687,16 +724,19 @@
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -708,16 +748,19 @@
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="H8" t="s">
-        <v>27</v>
+      <c r="H8" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -729,16 +772,19 @@
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="H9" t="s">
-        <v>23</v>
+      <c r="H9" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -750,16 +796,19 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="H10" t="s">
-        <v>25</v>
+      <c r="H10" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -771,16 +820,19 @@
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="H11" t="s">
-        <v>29</v>
+      <c r="H11" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5">
         <v>3</v>
@@ -792,16 +844,19 @@
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
-      <c r="H12" t="s">
-        <v>30</v>
+      <c r="H12" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -813,13 +868,13 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="H13" t="s">
-        <v>36</v>
+      <c r="H13" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -838,7 +893,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="7">
         <v>500</v>
@@ -846,7 +901,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -869,7 +924,7 @@
     </row>
     <row r="20" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -881,7 +936,20 @@
     </row>
     <row r="21" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{84C031F3-21DB-CC43-9833-4C44FD6F5222}"/>
+    <hyperlink ref="H10" r:id="rId2" xr:uid="{1DED8B49-E4C3-AE4C-ADCD-5EB46521D331}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{CC985303-985C-B94C-A712-FADD5F6E5063}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{F2F9C1EF-55A5-A140-8A1A-435944BDACA8}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{6F6A8BAA-B09B-484E-AAF1-3DBD043D89B9}"/>
+    <hyperlink ref="H5" r:id="rId6" xr:uid="{26273774-8742-024C-9653-C70DB190867D}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{368869DC-B761-CE4A-A26F-711FA86B3425}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{8F8478FB-4529-A54F-ACA0-CB867F783DA8}"/>
+    <hyperlink ref="H11" r:id="rId9" display="https://www.ebay.com/itm/Tarot-TL2D01-T2-2D-2-Axis-Brushless-Gimbal-PTZ-For-Gopro-Hero-4-3-3-FPV-Gimbal/282425843426?_trkparms=aid%3D555018%26algo%3DPL.SIM%26ao%3D1%26asc%3D20131003132420%26meid%3D3254323d803e48f082309082c086ad87%26pid%3D100005%26rk%3D1%26rkt%3D5%26sd%3D392133072686%26itm%3D282425843426&amp;_trksid=p2047675.c100005.m1851" xr:uid="{87A9083D-1184-5046-8AFB-113D48C567D3}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{0B6B4DC6-5F87-8D4A-B9FF-E83A13EBBA6A}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{E9613244-A90D-2E46-B306-C60C1CAA3F54}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>